<commit_message>
t&t game masters screen
</commit_message>
<xml_diff>
--- a/tunnels-trolls/checklist.xlsx
+++ b/tunnels-trolls/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/tunnels-trolls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687D5062-5240-2A4A-A2A2-EB02F78BFCEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B04204-E8DE-F945-BB7C-DDC208971E9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{37614222-0751-3546-BCA5-7171D6532E05}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{37614222-0751-3546-BCA5-7171D6532E05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
   <si>
     <t>year</t>
   </si>
@@ -189,6 +189,18 @@
   </si>
   <si>
     <t>Beyond the Wall of Tears</t>
+  </si>
+  <si>
+    <t>product_code</t>
+  </si>
+  <si>
+    <t>ゲームマスター・スクリーン</t>
+  </si>
+  <si>
+    <t>Gamemasters Screen</t>
+  </si>
+  <si>
+    <t>game_masters_screen.jpg</t>
   </si>
 </sst>
 </file>
@@ -549,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2E77AF-085C-CD47-A094-54C798EFE90E}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D15" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,7 +575,7 @@
     <col min="5" max="5" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,8 +594,11 @@
       <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1987</v>
       </c>
@@ -602,8 +617,11 @@
       <c r="F2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1988</v>
       </c>
@@ -623,7 +641,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1989</v>
       </c>
@@ -642,8 +660,11 @@
       <c r="F4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1991</v>
       </c>
@@ -662,8 +683,11 @@
       <c r="F5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1988</v>
       </c>
@@ -683,7 +707,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1990</v>
       </c>
@@ -702,8 +726,11 @@
       <c r="F7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1988</v>
       </c>
@@ -722,8 +749,11 @@
       <c r="F8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1988</v>
       </c>
@@ -742,8 +772,11 @@
       <c r="F9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1988</v>
       </c>
@@ -762,8 +795,11 @@
       <c r="F10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1989</v>
       </c>
@@ -782,8 +818,11 @@
       <c r="F11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1989</v>
       </c>
@@ -802,8 +841,11 @@
       <c r="F12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1990</v>
       </c>
@@ -822,8 +864,11 @@
       <c r="F13" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1990</v>
       </c>
@@ -842,8 +887,11 @@
       <c r="F14" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1991</v>
       </c>
@@ -861,6 +909,26 @@
       </c>
       <c r="F15" t="s">
         <v>49</v>
+      </c>
+      <c r="G15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more t&t product codes
</commit_message>
<xml_diff>
--- a/tunnels-trolls/checklist.xlsx
+++ b/tunnels-trolls/checklist.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/tunnels-trolls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B04204-E8DE-F945-BB7C-DDC208971E9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA1214A9-85DF-B543-8FEC-28986D6EFF3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{37614222-0751-3546-BCA5-7171D6532E05}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="checklist" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -564,7 +564,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:D16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,6 +640,9 @@
       <c r="F3" t="s">
         <v>48</v>
       </c>
+      <c r="G3">
+        <v>109</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -705,6 +708,9 @@
       </c>
       <c r="F6" t="s">
         <v>49</v>
+      </c>
+      <c r="G6">
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>